<commit_message>
Update parts list due to Amazon inventory change
Amazon removed the 3.2" display from the original link.  Do not use the 2.8" model.  3.2" can currently only be found with an included case.  The case isn't necessary, but is the only option as of 2/23/22.
</commit_message>
<xml_diff>
--- a/Origin Parts and Tools List.xlsx
+++ b/Origin Parts and Tools List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bacon\Documents\GitHub\Origin 2021-12-27 organized for public release\Origin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Arduino\Projects\Origin 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B322AFD-D3F4-4FEE-9244-A97B92DEE91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91574437-D792-466B-BC4B-E8F096450B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="960" windowWidth="29760" windowHeight="18255" xr2:uid="{D551B3D0-48E0-4B7F-B193-787E150CA982}"/>
+    <workbookView xWindow="9540" yWindow="1455" windowWidth="26355" windowHeight="17340" xr2:uid="{D551B3D0-48E0-4B7F-B193-787E150CA982}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
   <si>
     <t>Type</t>
   </si>
@@ -78,12 +78,6 @@
     <t>$25 for 10</t>
   </si>
   <si>
-    <t>Nextion Display - 3.2"</t>
-  </si>
-  <si>
-    <t>Nextion Display - 7"</t>
-  </si>
-  <si>
     <t>AC/DC Wall Mount Adapter 5V 20W</t>
   </si>
   <si>
@@ -277,6 +271,15 @@
   </si>
   <si>
     <t>$10 for 8</t>
+  </si>
+  <si>
+    <t>Nextion NX4024T032 Display - 3.2"</t>
+  </si>
+  <si>
+    <t>Nextion NX8048K070 Display - 7"</t>
+  </si>
+  <si>
+    <t>CASE IS NOT NEEDED, but Amazon is out of stock of just the display as of 2/23/22</t>
   </si>
 </sst>
 </file>
@@ -656,7 +659,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -689,7 +692,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -747,10 +750,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -758,10 +764,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -769,10 +775,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -780,13 +786,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -794,13 +800,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -808,13 +814,13 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -822,13 +828,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,13 +842,13 @@
         <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -850,13 +856,13 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -864,13 +870,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -878,13 +884,13 @@
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
         <v>35</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,13 +898,13 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
         <v>38</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -906,13 +912,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" t="s">
         <v>41</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -920,13 +926,13 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" t="s">
         <v>44</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -934,13 +940,13 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -948,13 +954,13 @@
         <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
         <v>49</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -962,13 +968,13 @@
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -976,13 +982,13 @@
         <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -990,112 +996,112 @@
         <v>3</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1111,7 @@
     <hyperlink ref="B4" r:id="rId3" display="https://www.amazon.com/Switch-Awakelion-Premium-Switcher-Support/dp/B06WV5YJ6H" xr:uid="{1235ED7F-24DC-4B39-9259-33B7F760B85D}"/>
     <hyperlink ref="B5" r:id="rId4" display="https://www.amazon.com/gp/product/B074HQQWD7" xr:uid="{4477E8F5-42D4-4363-8BB7-1C1C12147F3E}"/>
     <hyperlink ref="B6" r:id="rId5" display="https://www.amazon.com/gp/product/B074HGW2FC" xr:uid="{23390FA0-7036-48AC-899C-FBD83110BD4A}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://www.amazon.com/gp/product/B015DMOYHY" xr:uid="{6C85C689-3C46-4A3D-AE5B-F43D3073DB7A}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{6C85C689-3C46-4A3D-AE5B-F43D3073DB7A}"/>
     <hyperlink ref="B8" r:id="rId7" display="https://www.amazon.com/gp/product/B079177F98" xr:uid="{DB8DB61B-6C04-4622-A10C-060AD75B2135}"/>
     <hyperlink ref="B9" r:id="rId8" display="https://www.digikey.com/en/products/detail/cui-inc/SWI25-5-N-P5/7070092" xr:uid="{3A5405E1-650F-4EAA-92B3-7726CFD97DED}"/>
     <hyperlink ref="B10" r:id="rId9" display="https://www.digikey.com/en/products/detail/vishay-semiconductor-opto-division/TSOP34438/4074442" xr:uid="{7E4363E2-C1A2-4680-BD3C-155591AD1486}"/>

</xml_diff>